<commit_message>
included new xls file
</commit_message>
<xml_diff>
--- a/properties/testdata/KONEMobileSiteSurvey_TestData.xlsx
+++ b/properties/testdata/KONEMobileSiteSurvey_TestData.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\con_svijay02\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14520" windowHeight="3276"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6924" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Web_Login_Data" sheetId="3" r:id="rId1"/>
@@ -12,10 +17,9 @@
     <sheet name="-data-" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mobile_Data!$A$1:$E$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mobile_Data!$A$1:$D$70</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="143">
   <si>
     <t>Run_Browser</t>
   </si>
@@ -93,6 +97,9 @@
     <t>SF_Opportunity_Name</t>
   </si>
   <si>
+    <t>Atest_06062018</t>
+  </si>
+  <si>
     <t>No other comment</t>
   </si>
   <si>
@@ -451,9 +458,6 @@
   </si>
   <si>
     <t>Full</t>
-  </si>
-  <si>
-    <t>Atest_06062018</t>
   </si>
 </sst>
 </file>
@@ -871,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -905,12 +909,12 @@
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>142</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -928,7 +932,7 @@
         <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -951,11 +955,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -964,1197 +968,986 @@
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="49.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>117</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>116</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>115</v>
       </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
         <v>114</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>113</v>
       </c>
       <c r="D3">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" t="s">
         <v>108</v>
       </c>
-      <c r="D8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" t="s">
         <v>105</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>104</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>103</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
         <v>102</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>101</v>
       </c>
       <c r="D12">
         <v>15</v>
       </c>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D13">
         <v>1500</v>
       </c>
-      <c r="E13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D14">
         <v>10</v>
       </c>
-      <c r="E14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
       </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D16">
         <v>1500</v>
       </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D17">
         <v>2000</v>
       </c>
-      <c r="E17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D18">
         <v>1500</v>
       </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D19">
         <v>1800</v>
       </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
         <v>94</v>
       </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>93</v>
       </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
         <v>92</v>
-      </c>
-      <c r="E20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" t="s">
-        <v>91</v>
       </c>
       <c r="D21">
         <v>300</v>
       </c>
-      <c r="E21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D22">
         <v>310</v>
       </c>
-      <c r="E22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D23">
         <v>320</v>
       </c>
-      <c r="E23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
         <v>88</v>
-      </c>
-      <c r="B24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" t="s">
-        <v>87</v>
       </c>
       <c r="D24">
         <v>330</v>
       </c>
-      <c r="E24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
-      </c>
-      <c r="E25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
         <v>86</v>
       </c>
-      <c r="B27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>85</v>
       </c>
-      <c r="D27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
       </c>
-      <c r="E28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
       </c>
-      <c r="E29" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" t="s">
         <v>83</v>
       </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" t="s">
         <v>82</v>
       </c>
-      <c r="E30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>81</v>
       </c>
-      <c r="D31" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" t="s">
         <v>80</v>
       </c>
-      <c r="E31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>79</v>
       </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
         <v>78</v>
-      </c>
-      <c r="E32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" t="s">
-        <v>77</v>
       </c>
       <c r="D33" t="s">
         <v>2</v>
       </c>
-      <c r="E33" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D34" t="s">
         <v>2</v>
       </c>
-      <c r="E34" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D35" t="s">
         <v>2</v>
       </c>
-      <c r="E35" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D36" t="s">
         <v>2</v>
       </c>
-      <c r="E36" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D37" t="s">
         <v>2</v>
       </c>
-      <c r="E37" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" t="s">
         <v>74</v>
       </c>
-      <c r="B38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" t="s">
-        <v>75</v>
-      </c>
-      <c r="E38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>73</v>
       </c>
-      <c r="D39" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" t="s">
         <v>72</v>
       </c>
-      <c r="E39" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>71</v>
-      </c>
-      <c r="C40" t="s">
-        <v>70</v>
       </c>
       <c r="D40">
         <v>2009</v>
       </c>
-      <c r="E40" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
-      </c>
-      <c r="E41" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C42" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D42" t="s">
-        <v>137</v>
-      </c>
-      <c r="E42" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
       </c>
-      <c r="E43" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" t="s">
         <v>69</v>
       </c>
-      <c r="D44" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" t="s">
         <v>68</v>
       </c>
-      <c r="E44" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>67</v>
       </c>
-      <c r="D45" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" t="s">
         <v>66</v>
       </c>
-      <c r="E45" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>65</v>
       </c>
-      <c r="D46" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" t="s">
         <v>64</v>
-      </c>
-      <c r="E46" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" t="s">
-        <v>40</v>
-      </c>
-      <c r="C47" t="s">
-        <v>63</v>
       </c>
       <c r="D47">
         <v>2000</v>
       </c>
-      <c r="E47" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D48">
         <v>1200</v>
       </c>
-      <c r="E48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
       </c>
-      <c r="E49" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
       </c>
-      <c r="E50" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D51" t="s">
         <v>1</v>
       </c>
-      <c r="E51" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D52">
         <v>2200</v>
       </c>
-      <c r="E52" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" t="s">
         <v>57</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>56</v>
       </c>
-      <c r="D53" t="s">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" t="s">
         <v>55</v>
-      </c>
-      <c r="E53" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>51</v>
-      </c>
-      <c r="B54" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" t="s">
-        <v>54</v>
       </c>
       <c r="D54">
         <v>1200</v>
       </c>
-      <c r="E54" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D55">
         <v>15</v>
       </c>
-      <c r="E55" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D56">
         <v>50</v>
       </c>
-      <c r="E56" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" t="s">
         <v>51</v>
-      </c>
-      <c r="B57" t="s">
-        <v>40</v>
-      </c>
-      <c r="C57" t="s">
-        <v>50</v>
       </c>
       <c r="D57">
         <v>2000</v>
       </c>
-      <c r="E57" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C58" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D58" s="8" t="s">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" t="s">
         <v>48</v>
-      </c>
-      <c r="E58" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>46</v>
-      </c>
-      <c r="B59" t="s">
-        <v>40</v>
-      </c>
-      <c r="C59" t="s">
-        <v>47</v>
       </c>
       <c r="D59">
         <v>30</v>
       </c>
-      <c r="E59" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" t="s">
         <v>46</v>
-      </c>
-      <c r="B60" t="s">
-        <v>40</v>
-      </c>
-      <c r="C60" t="s">
-        <v>45</v>
       </c>
       <c r="D60">
         <v>150</v>
       </c>
-      <c r="E60" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B61" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" t="s">
         <v>44</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>43</v>
       </c>
-      <c r="D61" t="s">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>42</v>
       </c>
-      <c r="E61" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>41</v>
-      </c>
       <c r="B62" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" t="s">
         <v>40</v>
-      </c>
-      <c r="C62" t="s">
-        <v>39</v>
       </c>
       <c r="D62" t="s">
         <v>1</v>
       </c>
-      <c r="E62" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" t="s">
+        <v>39</v>
+      </c>
+      <c r="D63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" t="s">
+        <v>37</v>
+      </c>
+      <c r="D64" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>24</v>
+      </c>
+      <c r="B68" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" t="s">
+        <v>29</v>
+      </c>
+      <c r="D68" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>24</v>
+      </c>
+      <c r="B69" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70" t="s">
         <v>23</v>
-      </c>
-      <c r="B63" t="s">
-        <v>24</v>
-      </c>
-      <c r="C63" t="s">
-        <v>38</v>
-      </c>
-      <c r="D63" t="s">
-        <v>37</v>
-      </c>
-      <c r="E63" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>23</v>
-      </c>
-      <c r="B64" t="s">
-        <v>24</v>
-      </c>
-      <c r="C64" t="s">
-        <v>36</v>
-      </c>
-      <c r="D64" t="s">
-        <v>35</v>
-      </c>
-      <c r="E64" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>23</v>
-      </c>
-      <c r="B65" t="s">
-        <v>24</v>
-      </c>
-      <c r="C65" t="s">
-        <v>34</v>
-      </c>
-      <c r="D65" t="s">
-        <v>33</v>
-      </c>
-      <c r="E65" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>23</v>
-      </c>
-      <c r="B66" t="s">
-        <v>24</v>
-      </c>
-      <c r="C66" t="s">
-        <v>32</v>
-      </c>
-      <c r="D66" t="s">
-        <v>31</v>
-      </c>
-      <c r="E66" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>23</v>
-      </c>
-      <c r="B67" t="s">
-        <v>24</v>
-      </c>
-      <c r="C67" t="s">
-        <v>30</v>
-      </c>
-      <c r="D67" t="s">
-        <v>29</v>
-      </c>
-      <c r="E67" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>23</v>
-      </c>
-      <c r="B68" t="s">
-        <v>24</v>
-      </c>
-      <c r="C68" t="s">
-        <v>28</v>
-      </c>
-      <c r="D68" t="s">
-        <v>27</v>
-      </c>
-      <c r="E68" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>23</v>
-      </c>
-      <c r="B69" t="s">
-        <v>24</v>
-      </c>
-      <c r="C69" t="s">
-        <v>26</v>
-      </c>
-      <c r="D69" t="s">
-        <v>25</v>
-      </c>
-      <c r="E69" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70" t="s">
-        <v>24</v>
-      </c>
-      <c r="C70" t="s">
-        <v>23</v>
-      </c>
-      <c r="D70" t="s">
-        <v>22</v>
-      </c>
-      <c r="E70" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2162,7 +1955,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="297" yWindow="495" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="297" yWindow="495" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Section Data">
           <x14:formula1>
             <xm:f>'-data-'!$C$2:$C$12</xm:f>
@@ -2175,12 +1968,6 @@
           </x14:formula1>
           <xm:sqref>B2:B70</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Required field Data">
-          <x14:formula1>
-            <xm:f>'-data-'!$E$2:$E$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E70</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2192,7 +1979,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2213,16 +2000,16 @@
         <v>8</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>121</v>
-      </c>
       <c r="E1" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2233,16 +2020,16 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2253,25 +2040,25 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2279,10 +2066,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2290,10 +2077,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2301,10 +2088,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2312,7 +2099,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2320,22 +2107,22 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrate web and mobile tests to run end to end test
</commit_message>
<xml_diff>
--- a/properties/testdata/KONEMobileSiteSurvey_TestData.xlsx
+++ b/properties/testdata/KONEMobileSiteSurvey_TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\con_svijay02\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dung Bien\eclipse-workspace\mobilesitesurveytestautomation\properties\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{10A96085-BD18-4CE4-8EF7-B880F460317A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6924" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6924" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Web_Login_Data" sheetId="3" r:id="rId1"/>
@@ -17,9 +18,9 @@
     <sheet name="-data-" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mobile_Data!$A$1:$D$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mobile_Data!$A$1:$D$64</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="127">
   <si>
     <t>Run_Browser</t>
   </si>
@@ -401,54 +402,6 @@
   </si>
   <si>
     <t>Section</t>
-  </si>
-  <si>
-    <t>5 meters guide suitable</t>
-  </si>
-  <si>
-    <t>Car through-type</t>
-  </si>
-  <si>
-    <t>A-side Corridor illumination cabling</t>
-  </si>
-  <si>
-    <t>Switch on wall</t>
-  </si>
-  <si>
-    <t>r29 - Is the landing lighting sufficient</t>
-  </si>
-  <si>
-    <t>A-side Door full front</t>
-  </si>
-  <si>
-    <t>Retain landing doors (A-Side)</t>
-  </si>
-  <si>
-    <t>r36 - Fire rated landing doors</t>
-  </si>
-  <si>
-    <t>Concrete obstacle in shaft</t>
-  </si>
-  <si>
-    <t>Plumbing obstacle in shaft</t>
-  </si>
-  <si>
-    <t>Is the car balustrade adequate for dismantling</t>
-  </si>
-  <si>
-    <t>Main supply voltage</t>
-  </si>
-  <si>
-    <t>3x600V</t>
-  </si>
-  <si>
-    <t>Machine room location:</t>
-  </si>
-  <si>
-    <t>Adjacent</t>
-  </si>
-  <si>
-    <t>r19 - Is there safe access to machine and pulley room</t>
   </si>
   <si>
     <t>MSS_SelectPlannedTypes</t>
@@ -463,7 +416,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -872,7 +825,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -909,7 +862,7 @@
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -932,7 +885,7 @@
         <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -941,7 +894,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'-data-'!$F$2:$F$3</xm:f>
           </x14:formula1>
@@ -954,12 +907,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,7 +1043,7 @@
         <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -1101,27 +1054,27 @@
         <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1132,10 +1085,10 @@
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1146,10 +1099,10 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D13">
-        <v>1500</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1160,10 +1113,10 @@
         <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1171,13 +1124,13 @@
         <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="D15">
+        <v>2000</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1188,7 +1141,7 @@
         <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D16">
         <v>1500</v>
@@ -1202,10 +1155,10 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D17">
-        <v>2000</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1213,41 +1166,41 @@
         <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18">
-        <v>1500</v>
+        <v>94</v>
+      </c>
+      <c r="D18" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
         <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D19">
-        <v>1800</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="D20">
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1258,10 +1211,10 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D21">
-        <v>300</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1272,248 +1225,248 @@
         <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D22">
-        <v>310</v>
+        <v>330</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23">
-        <v>320</v>
+        <v>86</v>
+      </c>
+      <c r="D23" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24">
-        <v>330</v>
+        <v>84</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
         <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
         <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>130</v>
+        <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" t="s">
-        <v>83</v>
+        <v>71</v>
+      </c>
+      <c r="D30">
+        <v>2009</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
         <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D31" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
         <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
         <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D33" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>131</v>
-      </c>
-      <c r="D34" t="s">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="D34">
+        <v>2000</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
-      </c>
-      <c r="D35" t="s">
-        <v>2</v>
+        <v>63</v>
+      </c>
+      <c r="D35">
+        <v>1200</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
         <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>133</v>
+        <v>62</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
         <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>134</v>
+        <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
-      </c>
-      <c r="D39" t="s">
-        <v>73</v>
+        <v>59</v>
+      </c>
+      <c r="D39">
+        <v>2200</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1521,13 +1474,13 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40">
-        <v>2009</v>
+        <v>57</v>
+      </c>
+      <c r="D40" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1535,13 +1488,13 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>135</v>
-      </c>
-      <c r="D41" t="s">
-        <v>136</v>
+        <v>55</v>
+      </c>
+      <c r="D41">
+        <v>1200</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1549,13 +1502,13 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>137</v>
-      </c>
-      <c r="D42" t="s">
-        <v>138</v>
+        <v>54</v>
+      </c>
+      <c r="D42">
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1563,13 +1516,13 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
-      </c>
-      <c r="D43" t="s">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="D43">
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1577,80 +1530,80 @@
         <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" t="s">
-        <v>69</v>
+        <v>51</v>
+      </c>
+      <c r="D44">
+        <v>2000</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
         <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D45" t="s">
-        <v>67</v>
+        <v>50</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
-      </c>
-      <c r="D46" t="s">
-        <v>65</v>
+        <v>48</v>
+      </c>
+      <c r="D46">
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="D47">
-        <v>2000</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48">
-        <v>1200</v>
+        <v>44</v>
+      </c>
+      <c r="D48" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B49" t="s">
         <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
@@ -1658,295 +1611,113 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="D50" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B51" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D51" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>59</v>
-      </c>
-      <c r="D52">
-        <v>2200</v>
+        <v>35</v>
+      </c>
+      <c r="D52" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B53" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D53" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C54" t="s">
-        <v>55</v>
-      </c>
-      <c r="D54">
-        <v>1200</v>
+        <v>31</v>
+      </c>
+      <c r="D54" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B55" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C55" t="s">
-        <v>54</v>
-      </c>
-      <c r="D55">
-        <v>15</v>
+        <v>29</v>
+      </c>
+      <c r="D55" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C56" t="s">
-        <v>53</v>
-      </c>
-      <c r="D56">
-        <v>50</v>
+        <v>27</v>
+      </c>
+      <c r="D56" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C57" t="s">
-        <v>51</v>
-      </c>
-      <c r="D57">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>47</v>
-      </c>
-      <c r="B58" t="s">
-        <v>45</v>
-      </c>
-      <c r="C58" t="s">
-        <v>50</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>47</v>
-      </c>
-      <c r="B59" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" t="s">
-        <v>48</v>
-      </c>
-      <c r="D59">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>47</v>
-      </c>
-      <c r="B60" t="s">
-        <v>41</v>
-      </c>
-      <c r="C60" t="s">
-        <v>46</v>
-      </c>
-      <c r="D60">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>42</v>
-      </c>
-      <c r="B61" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" t="s">
-        <v>44</v>
-      </c>
-      <c r="D61" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>42</v>
-      </c>
-      <c r="B62" t="s">
-        <v>58</v>
-      </c>
-      <c r="C62" t="s">
-        <v>40</v>
-      </c>
-      <c r="D62" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
         <v>24</v>
       </c>
-      <c r="B63" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" t="s">
-        <v>39</v>
-      </c>
-      <c r="D63" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>24</v>
-      </c>
-      <c r="B64" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" t="s">
-        <v>37</v>
-      </c>
-      <c r="D64" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>24</v>
-      </c>
-      <c r="B65" t="s">
-        <v>25</v>
-      </c>
-      <c r="C65" t="s">
-        <v>35</v>
-      </c>
-      <c r="D65" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B66" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" t="s">
-        <v>33</v>
-      </c>
-      <c r="D66" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>24</v>
-      </c>
-      <c r="B67" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67" t="s">
-        <v>31</v>
-      </c>
-      <c r="D67" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>24</v>
-      </c>
-      <c r="B68" t="s">
-        <v>25</v>
-      </c>
-      <c r="C68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D68" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>24</v>
-      </c>
-      <c r="B69" t="s">
-        <v>25</v>
-      </c>
-      <c r="C69" t="s">
-        <v>27</v>
-      </c>
-      <c r="D69" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" t="s">
-        <v>25</v>
-      </c>
-      <c r="C70" t="s">
-        <v>24</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="D57" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1956,17 +1727,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="297" yWindow="495" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Section Data">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Section Data" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'-data-'!$C$2:$C$12</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A70</xm:sqref>
+          <xm:sqref>A2:A64</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Type Data">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Type Data" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'-data-'!$D$2:$D$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B70</xm:sqref>
+          <xm:sqref>B2:B64</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1975,7 +1746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2009,7 +1780,7 @@
         <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2029,7 +1800,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2049,7 +1820,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added latest excel file and the modification in excel is added a sheet named Login_Data for user Credentials
</commit_message>
<xml_diff>
--- a/properties/testdata/KONEMobileSiteSurvey_TestData.xlsx
+++ b/properties/testdata/KONEMobileSiteSurvey_TestData.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dung Bien\eclipse-workspace\mobilesitesurveytestautomation\properties\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\con_svijay02\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{10A96085-BD18-4CE4-8EF7-B880F460317A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6924" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6924"/>
   </bookViews>
   <sheets>
-    <sheet name="Web_Login_Data" sheetId="3" r:id="rId1"/>
-    <sheet name="Mobile_Data" sheetId="4" r:id="rId2"/>
-    <sheet name="-data-" sheetId="2" r:id="rId3"/>
+    <sheet name="Login_Data" sheetId="5" r:id="rId1"/>
+    <sheet name="Web_Login_Data" sheetId="3" r:id="rId2"/>
+    <sheet name="Mobile_Data" sheetId="4" r:id="rId3"/>
+    <sheet name="-data-" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mobile_Data!$A$1:$D$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mobile_Data!$A$1:$D$64</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="135">
   <si>
     <t>Run_Browser</t>
   </si>
@@ -83,24 +83,9 @@
     <t>MSS_City</t>
   </si>
   <si>
-    <t>ATEST_CustomerContact</t>
-  </si>
-  <si>
-    <t>ATEST_Street</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>ATEST_City</t>
-  </si>
-  <si>
     <t>SF_Opportunity_Name</t>
   </si>
   <si>
-    <t>Atest_06062018</t>
-  </si>
-  <si>
     <t>No other comment</t>
   </si>
   <si>
@@ -411,12 +396,51 @@
   </si>
   <si>
     <t>Full</t>
+  </si>
+  <si>
+    <t>SF_UserName</t>
+  </si>
+  <si>
+    <t>SF_Password</t>
+  </si>
+  <si>
+    <t>Site_UserName</t>
+  </si>
+  <si>
+    <t>Site_Password</t>
+  </si>
+  <si>
+    <t>b.mamtha@kone.com</t>
+  </si>
+  <si>
+    <t>Data@123</t>
+  </si>
+  <si>
+    <t>con_bmamtha</t>
+  </si>
+  <si>
+    <t>Welcome@123</t>
+  </si>
+  <si>
+    <t>Atest_06062018_1</t>
+  </si>
+  <si>
+    <t>ATEST_CustomerContact_2106</t>
+  </si>
+  <si>
+    <t>ATEST_Street_2106</t>
+  </si>
+  <si>
+    <t>21062018</t>
+  </si>
+  <si>
+    <t>ATEST_City_2106</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -499,7 +523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -511,6 +535,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -825,12 +850,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -844,7 +915,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
@@ -862,30 +933,30 @@
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>131</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -894,7 +965,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'-data-'!$F$2:$F$3</xm:f>
           </x14:formula1>
@@ -906,13 +977,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -925,41 +996,41 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D3">
         <v>13</v>
@@ -967,13 +1038,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
@@ -981,13 +1052,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -995,13 +1066,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
         <v>106</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" t="s">
-        <v>111</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
@@ -1009,13 +1080,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
@@ -1023,27 +1094,27 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -1051,27 +1122,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D11">
         <v>15</v>
@@ -1079,13 +1150,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D12">
         <v>1500</v>
@@ -1093,13 +1164,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
         <v>95</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>100</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -1107,13 +1178,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D14">
         <v>1500</v>
@@ -1121,13 +1192,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D15">
         <v>2000</v>
@@ -1135,13 +1206,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D16">
         <v>1500</v>
@@ -1149,13 +1220,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D17">
         <v>1800</v>
@@ -1163,27 +1234,27 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D19">
         <v>300</v>
@@ -1191,13 +1262,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D20">
         <v>310</v>
@@ -1205,13 +1276,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D21">
         <v>320</v>
@@ -1219,13 +1290,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D22">
         <v>330</v>
@@ -1233,69 +1304,69 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
         <v>75</v>
       </c>
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" t="s">
-        <v>80</v>
-      </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
         <v>2</v>
@@ -1303,41 +1374,41 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D30">
         <v>2009</v>
@@ -1345,55 +1416,55 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D34">
         <v>2000</v>
@@ -1401,13 +1472,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D35">
         <v>1200</v>
@@ -1415,13 +1486,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
@@ -1429,13 +1500,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
@@ -1443,13 +1514,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
@@ -1457,13 +1528,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D39">
         <v>2200</v>
@@ -1471,27 +1542,27 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="s">
         <v>52</v>
       </c>
-      <c r="B40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" t="s">
-        <v>57</v>
-      </c>
       <c r="D40" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D41">
         <v>1200</v>
@@ -1499,13 +1570,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D42">
         <v>15</v>
@@ -1513,13 +1584,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D43">
         <v>50</v>
@@ -1527,13 +1598,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D44">
         <v>2000</v>
@@ -1541,27 +1612,27 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
         <v>45</v>
       </c>
-      <c r="C45" t="s">
-        <v>50</v>
-      </c>
       <c r="D45" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C46" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D46">
         <v>30</v>
@@ -1569,13 +1640,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" t="s">
         <v>41</v>
-      </c>
-      <c r="C47" t="s">
-        <v>46</v>
       </c>
       <c r="D47">
         <v>150</v>
@@ -1583,27 +1654,27 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D48" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
@@ -1611,114 +1682,114 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D50" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C51" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D51" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C52" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D52" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B53" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D53" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" t="s">
         <v>25</v>
-      </c>
-      <c r="C54" t="s">
-        <v>31</v>
-      </c>
-      <c r="D54" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s">
         <v>24</v>
       </c>
-      <c r="B55" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" t="s">
-        <v>29</v>
-      </c>
       <c r="D55" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D56" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C57" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D57" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1727,13 +1798,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="297" yWindow="495" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Section Data" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Section Data">
           <x14:formula1>
             <xm:f>'-data-'!$C$2:$C$12</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A64</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Type Data" xr:uid="{00000000-0002-0000-0100-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Type Data">
           <x14:formula1>
             <xm:f>'-data-'!$D$2:$D$7</xm:f>
           </x14:formula1>
@@ -1745,8 +1816,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1771,16 +1842,16 @@
         <v>8</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1791,16 +1862,16 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1811,25 +1882,25 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1837,10 +1908,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1848,10 +1919,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1859,10 +1930,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1870,7 +1941,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1878,22 +1949,22 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>